<commit_message>
Basic Error detection. needs more work
</commit_message>
<xml_diff>
--- a/Testing/Excel_File.xlsx
+++ b/Testing/Excel_File.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067E7DA4-E7B9-430E-9512-A8A7CA606069}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8173A7D6-1345-4449-A499-BF7C64810658}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33570" yWindow="1185" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36000" yWindow="2100" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Col 1</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Britt</t>
   </si>
   <si>
-    <t>admin</t>
-  </si>
-  <si>
     <t>Eric</t>
   </si>
   <si>
@@ -61,10 +58,10 @@
     <t>Col 5</t>
   </si>
   <si>
-    <t>Col 6</t>
-  </si>
-  <si>
     <t>asdf</t>
+  </si>
+  <si>
+    <t>admin1</t>
   </si>
   <si>
     <t>jhgf</t>
@@ -414,7 +411,7 @@
   <dimension ref="E5:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,11 +430,9 @@
         <v>3</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="J5" s="1"/>
     </row>
     <row r="6" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E6" s="1" t="s">
@@ -447,7 +442,7 @@
         <v>5</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H6" s="1">
         <v>12345</v>
@@ -456,18 +451,18 @@
         <v>12345</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H7" s="1">
         <v>54321</v>
@@ -476,7 +471,7 @@
         <v>643353</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="5:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added some more basic error detections. Still needs some work, but basic things work. Checks for this -Correct Num of rows -Each column has name -Column is correct name
</commit_message>
<xml_diff>
--- a/Testing/Excel_File.xlsx
+++ b/Testing/Excel_File.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35574704-0C1D-420B-A786-D83515FC5F7A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D66A67-A8D6-4291-85A7-0C90568C85DF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35850" yWindow="2625" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7395" yWindow="720" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
-  <si>
-    <t>Col 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Dillon</t>
   </si>
@@ -37,37 +34,25 @@
     <t>Eric</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>something</t>
-  </si>
-  <si>
-    <t>abb</t>
-  </si>
-  <si>
-    <t>Col 4</t>
-  </si>
-  <si>
-    <t>Col 6</t>
-  </si>
-  <si>
-    <t>asg</t>
-  </si>
-  <si>
-    <t>sdfg</t>
-  </si>
-  <si>
-    <t>asdg</t>
-  </si>
-  <si>
-    <t>asdf</t>
-  </si>
-  <si>
-    <t>Col 3</t>
-  </si>
-  <si>
-    <t>tes</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>First_Name</t>
+  </si>
+  <si>
+    <t>Last_Name</t>
+  </si>
+  <si>
+    <t>Britt</t>
+  </si>
+  <si>
+    <t>Claus</t>
+  </si>
+  <si>
+    <t>Noelia</t>
+  </si>
+  <si>
+    <t>Oase</t>
   </si>
 </sst>
 </file>
@@ -414,30 +399,28 @@
   <dimension ref="E5:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="5" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E5" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -445,22 +428,18 @@
       <c r="O5" s="1"/>
     </row>
     <row r="6" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1"/>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="G6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -468,28 +447,35 @@
       <c r="O6" s="1"/>
     </row>
     <row r="7" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E7" s="1" t="s">
-        <v>2</v>
+      <c r="E7" s="1">
+        <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
+    <row r="8" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="9" spans="5:15" x14ac:dyDescent="0.25">
       <c r="M9" s="2"/>
     </row>

</xml_diff>

<commit_message>
Revert "Revert "allow null""
This reverts commit 88b693329fb93d68f76825cbee14251a6f3e3bdf.
</commit_message>
<xml_diff>
--- a/Testing/Excel_File.xlsx
+++ b/Testing/Excel_File.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D66A67-A8D6-4291-85A7-0C90568C85DF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C39DB1B-9090-4C4D-ACA0-D553F01ABD76}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7395" yWindow="720" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="720" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,40 +26,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Dillon</t>
-  </si>
-  <si>
-    <t>Eric</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>First_Name</t>
-  </si>
-  <si>
-    <t>Last_Name</t>
-  </si>
-  <si>
-    <t>Britt</t>
-  </si>
-  <si>
-    <t>Claus</t>
-  </si>
-  <si>
-    <t>Noelia</t>
-  </si>
-  <si>
-    <t>Oase</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>adf</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>asdfba</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>atadd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,14 +66,6 @@
       <color rgb="FF242729"/>
       <name val="Consolas"/>
       <family val="3"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,11 +85,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -111,12 +96,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -396,10 +377,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="E5:O13"/>
+  <dimension ref="B4:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B4" sqref="B4:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,79 +389,54 @@
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E5" s="1" t="s">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="G5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-    </row>
-    <row r="7" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-    </row>
-    <row r="8" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E8" s="1">
-        <v>2</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M9" s="2"/>
     </row>
-    <row r="13" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="J13" s="3"/>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="P12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished up with sprint 1
</commit_message>
<xml_diff>
--- a/Testing/Excel_File.xlsx
+++ b/Testing/Excel_File.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C39DB1B-9090-4C4D-ACA0-D553F01ABD76}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1DF9EE-5EAE-4BFB-93F9-0C6B03A021C6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="720" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,27 +26,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
-  <si>
-    <t>asdf</t>
-  </si>
-  <si>
-    <t>adf</t>
-  </si>
-  <si>
-    <t>test3</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>asdfba</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>atadd</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Dillon</t>
+  </si>
+  <si>
+    <t>Britt</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Test2</t>
+  </si>
+  <si>
+    <t>Test5</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>First_Name</t>
+  </si>
+  <si>
+    <t>Last_Name5</t>
   </si>
 </sst>
 </file>
@@ -380,7 +386,7 @@
   <dimension ref="B4:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:G5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,38 +396,57 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" t="s">
+        <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="G5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M9" s="2"/>

</xml_diff>